<commit_message>
Update part list, added SCPI code from Dean, made a lazy circular buffer for usb commands
</commit_message>
<xml_diff>
--- a/Alternate Part List.xlsx
+++ b/Alternate Part List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krotain\Documents\git\493\ece_492-3_topic_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E72F08-9D5A-4E49-92B0-E7807DF91F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0590627A-8135-4BDF-8AA6-0478945E325C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2175" windowWidth="29040" windowHeight="16440" xr2:uid="{DD9C814F-33BB-46B4-954A-62ACB4677A0F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="177">
   <si>
     <t>Part(*=Similar)</t>
   </si>
@@ -561,6 +561,12 @@
   </si>
   <si>
     <t>0.2Ohm</t>
+  </si>
+  <si>
+    <t>3083et</t>
+  </si>
+  <si>
+    <t>Front Panel Keys</t>
   </si>
 </sst>
 </file>
@@ -943,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABF4B5B-D5F0-478D-961E-5722ED7FBC19}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1025,7 @@
       </c>
       <c r="J2">
         <f>SUM(E:E)</f>
-        <v>97.884170000000026</v>
+        <v>106.07417000000002</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1605,9 +1611,8 @@
       <c r="D22">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E22">
-        <f t="shared" ref="E22:E29" si="3">D22*B22</f>
-        <v>0.56999999999999995</v>
+      <c r="E22" t="s">
+        <v>175</v>
       </c>
       <c r="F22" t="s">
         <v>174</v>
@@ -1636,7 +1641,7 @@
         <v>0.38736999999999999</v>
       </c>
       <c r="E23">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E22:E29" si="3">D23*B23</f>
         <v>0.77473999999999998</v>
       </c>
       <c r="F23" t="s">
@@ -1693,11 +1698,11 @@
         <v>6.41</v>
       </c>
       <c r="D25">
-        <v>3.41</v>
+        <v>7.29</v>
       </c>
       <c r="E25">
         <f t="shared" si="3"/>
-        <v>6.82</v>
+        <v>14.58</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
@@ -2686,6 +2691,32 @@
       </c>
       <c r="I58" s="3" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>176</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>